<commit_message>
populate names of students and lecutures and other things
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\الدنيا\Computer Science\1testOfProjectGraduation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7465E84E-6899-4F97-AD22-AD9D4D98D909}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C670B9-4E1C-4B77-8503-E71F6311530C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{09F5FF17-1189-4AF3-8B48-C2019F03BAE0}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>CS</t>
   </si>
@@ -48,21 +48,12 @@
     <t>password</t>
   </si>
   <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>student</t>
-  </si>
-  <si>
     <t>level</t>
   </si>
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>deparment</t>
-  </si>
-  <si>
     <t>semester</t>
   </si>
   <si>
@@ -88,6 +79,18 @@
   </si>
   <si>
     <t>AI</t>
+  </si>
+  <si>
+    <t>Eslam</t>
+  </si>
+  <si>
+    <t>eslam@e.com</t>
+  </si>
+  <si>
+    <t>pass33</t>
+  </si>
+  <si>
+    <t>department</t>
   </si>
 </sst>
 </file>
@@ -450,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{377BB9D3-316E-470C-A828-8DF68D4DE0E1}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -462,11 +465,11 @@
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
     <col min="3" max="3" width="17.21875" customWidth="1"/>
     <col min="4" max="4" width="16.44140625" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="9" max="9" width="30.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -474,30 +477,27 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="B2" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -505,25 +505,22 @@
       <c r="D2">
         <v>2282</v>
       </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2">
+      <c r="E2">
         <v>20340</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" t="s">
         <v>0</v>
       </c>
-      <c r="H2">
+      <c r="G2">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -531,43 +528,60 @@
       <c r="D3">
         <v>2282</v>
       </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3">
+      <c r="E3">
         <v>20345</v>
       </c>
-      <c r="G3" t="s">
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <v>20344</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5">
+        <v>204050</v>
+      </c>
+      <c r="F5" t="s">
         <v>1</v>
       </c>
-      <c r="H3">
+      <c r="G5">
         <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4">
-        <v>20344</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -575,6 +589,7 @@
     <hyperlink ref="B2" r:id="rId1" xr:uid="{CF4C1A4C-31C7-4062-BA3B-D3C487F91AD6}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{84AF3A99-2E36-4D9D-819E-8D1EF9FD4BFC}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{33A3DD29-E079-4CD6-A5B8-EED7BB9D01D3}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{A82508D3-C965-435F-9B48-42C5F53DBCE4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
access to user and student to create attendance
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\الدنيا\Computer Science\1testOfProjectGraduation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C670B9-4E1C-4B77-8503-E71F6311530C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6F21DA-D3AF-46ED-9993-50D863E1158D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{09F5FF17-1189-4AF3-8B48-C2019F03BAE0}"/>
   </bookViews>
@@ -57,40 +57,40 @@
     <t>semester</t>
   </si>
   <si>
-    <t>arafa</t>
-  </si>
-  <si>
-    <t>nabil</t>
-  </si>
-  <si>
-    <t>ar@ee.com</t>
-  </si>
-  <si>
-    <t>na@ee.com</t>
-  </si>
-  <si>
-    <t>omar</t>
-  </si>
-  <si>
-    <t>omar@o.com</t>
-  </si>
-  <si>
     <t>23ii</t>
   </si>
   <si>
     <t>AI</t>
   </si>
   <si>
-    <t>Eslam</t>
-  </si>
-  <si>
-    <t>eslam@e.com</t>
-  </si>
-  <si>
     <t>pass33</t>
   </si>
   <si>
     <t>department</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>i@ee.com</t>
+  </si>
+  <si>
+    <t>b@ee.com</t>
+  </si>
+  <si>
+    <t>c@o.com</t>
+  </si>
+  <si>
+    <t>d@e.com</t>
   </si>
 </sst>
 </file>
@@ -456,7 +456,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,7 +486,7 @@
         <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
         <v>7</v>
@@ -494,10 +494,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -517,10 +517,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -540,22 +540,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E4">
         <v>20344</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G4">
         <v>8</v>
@@ -563,16 +563,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E5">
         <v>204050</v>

</xml_diff>

<commit_message>
report of staff and doctor
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\الدنيا\Computer Science\1testOfProjectGraduation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97131A21-CA08-45DE-9C38-DA0CBF852389}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3021B71C-F3E9-4313-919F-0B304D28E8D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{09F5FF17-1189-4AF3-8B48-C2019F03BAE0}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>CS</t>
   </si>
@@ -51,43 +51,40 @@
     <t>level</t>
   </si>
   <si>
-    <t>23ii</t>
-  </si>
-  <si>
     <t>AI</t>
   </si>
   <si>
-    <t>pass33</t>
-  </si>
-  <si>
     <t>department</t>
   </si>
   <si>
     <t>passwordConfirm</t>
   </si>
   <si>
-    <t>iiiii</t>
-  </si>
-  <si>
-    <t>bbbb</t>
-  </si>
-  <si>
-    <t>ccccc</t>
-  </si>
-  <si>
-    <t>ddddd</t>
-  </si>
-  <si>
-    <t>ii@ee.com</t>
-  </si>
-  <si>
-    <t>bb@ee.com</t>
-  </si>
-  <si>
-    <t>cc@o.com</t>
-  </si>
-  <si>
-    <t>dd@e.com</t>
+    <t>aliii</t>
+  </si>
+  <si>
+    <t>stt1@ee.com</t>
+  </si>
+  <si>
+    <t>stt1</t>
+  </si>
+  <si>
+    <t>stt111</t>
+  </si>
+  <si>
+    <t>stt11</t>
+  </si>
+  <si>
+    <t>stt11@o.com</t>
+  </si>
+  <si>
+    <t>stt111@e.com</t>
+  </si>
+  <si>
+    <t>ali12@ee.com</t>
+  </si>
+  <si>
+    <t>pass22</t>
   </si>
 </sst>
 </file>
@@ -461,7 +458,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,28 +486,28 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>4</v>
       </c>
-      <c r="D2">
-        <v>2282</v>
-      </c>
-      <c r="E2">
-        <v>2282</v>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -518,19 +515,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
-      <c r="D3">
-        <v>2282</v>
-      </c>
-      <c r="E3">
-        <v>2282</v>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
       </c>
       <c r="F3" t="s">
         <v>0</v>
@@ -541,36 +538,36 @@
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>4</v>
       </c>
       <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
         <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
         <v>1</v>

</xml_diff>